<commit_message>
Fixed bug when config field was there but empty
</commit_message>
<xml_diff>
--- a/config/images.xlsx
+++ b/config/images.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreaverlicchi/Code/responsive-images-automator/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7882A318-6886-FA41-96F7-C380290E8300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501F33AB-2668-8C43-9689-4353FC029B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21460" yWindow="7400" windowWidth="16940" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11840" yWindow="7400" windowWidth="16940" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="extraction" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>pageName</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>imageTemplate</t>
-  </si>
-  <si>
-    <t>https://web-dev.imgix.net/image/8WbTDNrhLsU0El80frMBGE4eMCD3/CZo4R87iOBYiRpIq6NcP.jpg?auto=format&amp;w={{ width }}</t>
   </si>
   <si>
     <t>webdev-mishipay</t>
@@ -113,11 +110,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -340,7 +338,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -375,16 +373,14 @@
       <c r="D2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -392,16 +388,12 @@
       <c r="D3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="E3" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{986AC67A-66CD-1D4B-87B0-7745FCF0C716}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{74D8A320-68CA-884A-B3F2-35EF3E2E5703}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>